<commit_message>
Got adj test passing
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whmeinert\CLionProjects\Eclipse\ClueProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\eclipse-workspace\ClueProject\ClueProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DD77193D-F182-4DAC-8C37-3A326C9DD621}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BABA52-B8D3-4016-AB25-3B9D8F5CC174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{64EDCF6C-983A-4D65-9789-1C28D60B590E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EDCF6C-983A-4D65-9789-1C28D60B590E}"/>
   </bookViews>
   <sheets>
     <sheet name="ClueLayout" sheetId="1" r:id="rId1"/>
@@ -529,15 +529,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1117CA6-8353-400F-B70D-2A55AE2B062B}">
-  <dimension ref="B2:Z28"/>
+  <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -614,7 +694,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -691,7 +774,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -768,7 +854,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -845,7 +934,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -922,7 +1014,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
@@ -999,7 +1094,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1174,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
@@ -1153,7 +1254,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1334,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1414,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1384,7 +1494,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1574,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1538,7 +1654,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1615,7 +1734,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1692,7 +1814,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1769,7 +1894,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1846,7 +1974,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1923,7 +2054,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
@@ -2000,7 +2134,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
@@ -2077,7 +2214,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
       <c r="B22" s="4" t="s">
         <v>1</v>
       </c>
@@ -2154,7 +2294,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>0</v>
       </c>
@@ -2231,7 +2374,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
@@ -2308,7 +2454,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
@@ -2385,7 +2534,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
       <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
@@ -2462,7 +2614,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
@@ -2539,7 +2694,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>